<commit_message>
Timeseries Gen and Spatial Nodes
Time series for the CBC file have been generated for all of the CDEC reservoirs. They just need to be combined with the existing data now. For the CBC specs file, existing reservoir data remaining unchanged. New reservoir data being added with combo of script and manual process (manually, adjusting gw nodes that fall outside NHD polygon, but seem in/close to reservoir per imagery review).
</commit_message>
<xml_diff>
--- a/Constrained_Head_BC/Code/cdec_reservoirs.xlsx
+++ b/Constrained_Head_BC/Code/cdec_reservoirs.xlsx
@@ -59,12 +59,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
       <name val="Tahoma"/>
       <family val="2"/>
       <color indexed="81"/>
@@ -76,6 +70,12 @@
       <b val="1"/>
       <color indexed="81"/>
       <sz val="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -148,7 +148,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -241,6 +241,12 @@
       <text>
         <t>Anchor, Nicholas@DWR:
 Manually input for now</t>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0">
+      <text>
+        <t>Anchor, Nicholas@DWR:
+Changed to code 15 and monthly due to longer record</t>
       </text>
     </comment>
     <comment ref="A9" authorId="0" shapeId="0">
@@ -545,7 +551,7 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -656,7 +662,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>6: RES ELE</t>
+          <t>15: STORAGE</t>
         </is>
       </c>
       <c r="D4">
@@ -669,7 +675,7 @@
       </c>
       <c r="F4" s="1" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>M</t>
         </is>
       </c>
       <c r="G4">

</xml_diff>

<commit_message>
Spec and Timeseries CSVs Generated
Updated CBC specification and timeseries CSVs generated in the code\output folder. Lakebed conductance seems incorrect, need to investigate.
</commit_message>
<xml_diff>
--- a/Constrained_Head_BC/Code/cdec_reservoirs.xlsx
+++ b/Constrained_Head_BC/Code/cdec_reservoirs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nanchor\Documents\GitHub\C2VSimFGv2.0_surface_water\Constrained_Head_BC\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D95DF9E-D65D-464A-81A1-3000F638B74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D2D609-F02A-43F6-B530-1DAF68BC5C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>